<commit_message>
Räumt die Auswertungen auf
</commit_message>
<xml_diff>
--- a/Hochschulstatistiken.xlsx
+++ b/Hochschulstatistiken.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achim\Desktop\Proj Hochschulfinanzierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF4284C-F2D2-4D90-8CC2-402B7ACE4713}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746D1206-D8CF-430B-8DF2-3ECDAFE7CDC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ZWISCHEN" sheetId="1" r:id="rId1"/>
@@ -1076,30 +1076,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">2018 -&gt; 2019 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Steigerung Professorenstellen [BW]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">2009 -&gt; 2019
 </t>
     </r>
@@ -1352,6 +1328,30 @@
       <t xml:space="preserve">
 Steigerung 
 Einnahmen Beiträge Studierende</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2000 -&gt; 2019 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Steigerung Professorenstellen [BW]</t>
     </r>
   </si>
 </sst>
@@ -6924,10 +6924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S94"/>
+  <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="F24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6997,7 +6997,7 @@
         <v>313</v>
       </c>
       <c r="P4" s="80" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
@@ -7227,7 +7227,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
         <v>297</v>
       </c>
@@ -7249,7 +7249,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>124</v>
       </c>
@@ -7263,7 +7263,7 @@
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>2019</v>
       </c>
@@ -7295,7 +7295,7 @@
         <v>149890</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>2018</v>
       </c>
@@ -7327,7 +7327,7 @@
         <v>131760</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>125</v>
       </c>
@@ -7341,7 +7341,7 @@
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>2019</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>2018</v>
       </c>
@@ -7405,15 +7405,15 @@
         <v>3614</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:16" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A26" s="56" t="s">
         <v>306</v>
       </c>
       <c r="B26" s="57"/>
       <c r="C26" s="57"/>
     </row>
-    <row r="28" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B29" s="12" t="s">
         <v>250</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" s="12" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
         <v>103</v>
@@ -7442,16 +7442,25 @@
         <v>300</v>
       </c>
       <c r="J30" s="41" t="s">
+        <v>325</v>
+      </c>
+      <c r="K30" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="K30" s="41" t="s">
+      <c r="L30" s="53" t="s">
         <v>315</v>
       </c>
-      <c r="L30" s="53" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="N30" s="59" t="s">
+        <v>300</v>
+      </c>
+      <c r="O30" s="44" t="s">
+        <v>323</v>
+      </c>
+      <c r="P30" s="28" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>2000</v>
       </c>
@@ -7485,8 +7494,19 @@
         <f>(C50/C49)-1</f>
         <v>-2.0840450973693248E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="N31" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="O31" s="73">
+        <f>(168671/114993)-1</f>
+        <v>0.46679363091666448</v>
+      </c>
+      <c r="P31" s="76">
+        <f>1-(171645/168671)</f>
+        <v>-1.7631958072223508E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>2001</v>
       </c>
@@ -7520,6 +7540,17 @@
         <f>(D50/D49)-1</f>
         <v>1.9073569482288777E-2</v>
       </c>
+      <c r="N32" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="O32" s="74">
+        <f>(24923/15029)-1</f>
+        <v>0.6583272340142392</v>
+      </c>
+      <c r="P32" s="75">
+        <f>(24923/24195)-1</f>
+        <v>3.0088861334986561E-2</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
@@ -8518,30 +8549,21 @@
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="G77" s="13"/>
     </row>
-    <row r="82" spans="4:19" ht="58" x14ac:dyDescent="0.35">
+    <row r="82" spans="4:7" ht="58" x14ac:dyDescent="0.35">
       <c r="D82" s="59" t="s">
         <v>305</v>
       </c>
       <c r="E82" s="41" t="s">
+        <v>320</v>
+      </c>
+      <c r="F82" s="41" t="s">
         <v>321</v>
       </c>
-      <c r="F82" s="41" t="s">
-        <v>322</v>
-      </c>
       <c r="G82" s="48" t="s">
-        <v>318</v>
-      </c>
-      <c r="Q82" s="59" t="s">
-        <v>300</v>
-      </c>
-      <c r="R82" s="44" t="s">
-        <v>324</v>
-      </c>
-      <c r="S82" s="28" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="83" spans="4:19" x14ac:dyDescent="0.35">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="83" spans="4:7" x14ac:dyDescent="0.35">
       <c r="D83" s="35" t="s">
         <v>124</v>
       </c>
@@ -8557,19 +8579,8 @@
         <f>(F83/E83)-1</f>
         <v>8.570304338026058E-2</v>
       </c>
-      <c r="Q83" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="R83" s="73">
-        <f>(168671/114993)-1</f>
-        <v>0.46679363091666448</v>
-      </c>
-      <c r="S83" s="76">
-        <f>1-(171645/168671)</f>
-        <v>-1.7631958072223508E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="4:19" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="4:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D84" s="23" t="s">
         <v>125</v>
       </c>
@@ -8585,39 +8596,28 @@
         <f>(F84/E84)-1</f>
         <v>1.9701867147132734E-2</v>
       </c>
-      <c r="Q84" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="R84" s="74">
-        <f>(24923/15029)-1</f>
-        <v>0.6583272340142392</v>
-      </c>
-      <c r="S84" s="75">
-        <f>(24923/24195)-1</f>
-        <v>3.0088861334986561E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="4:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="4:7" x14ac:dyDescent="0.35">
       <c r="D85" s="33"/>
       <c r="E85" s="20"/>
       <c r="F85" s="20"/>
       <c r="G85" s="49"/>
     </row>
-    <row r="86" spans="4:19" ht="58" x14ac:dyDescent="0.35">
+    <row r="86" spans="4:7" ht="58" x14ac:dyDescent="0.35">
       <c r="D86" s="58" t="s">
         <v>305</v>
       </c>
       <c r="E86" s="47" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F86" s="47" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G86" s="50" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="87" spans="4:19" x14ac:dyDescent="0.35">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="87" spans="4:7" x14ac:dyDescent="0.35">
       <c r="D87" s="35" t="s">
         <v>124</v>
       </c>
@@ -8634,7 +8634,7 @@
         <v>6.2672928807161243E-2</v>
       </c>
     </row>
-    <row r="88" spans="4:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="88" spans="4:7" ht="29" x14ac:dyDescent="0.35">
       <c r="D88" s="25" t="s">
         <v>125</v>
       </c>
@@ -8651,7 +8651,7 @@
         <v>3.6480959164509219E-2</v>
       </c>
     </row>
-    <row r="94" spans="4:19" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="94" spans="4:7" ht="29" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B55:C55"/>

</xml_diff>

<commit_message>
Ändert den Zeitstempel der Datei
</commit_message>
<xml_diff>
--- a/Hochschulstatistiken.xlsx
+++ b/Hochschulstatistiken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Achim\Desktop\Proj Hochschulfinanzierung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746D1206-D8CF-430B-8DF2-3ECDAFE7CDC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B00A7FD-9519-451B-9C16-F5A8FED1B4EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6926,8 +6926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q37" sqref="Q37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>